<commit_message>
[Exercise 8] Extention with extend
</commit_message>
<xml_diff>
--- a/week-7/oop_mind_map_delux_ultra_premium.xlsx
+++ b/week-7/oop_mind_map_delux_ultra_premium.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@dev\@education\java-intro-2019-2020\week-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A72035-A00B-4BC0-925D-47A463D389A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088E24FF-B3FD-4107-969D-33E64A76CC56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{91A0B163-A117-473A-BDB9-98CB62830661}"/>
   </bookViews>
@@ -130,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,21 +183,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,46 +515,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533F0A5A-5C62-4542-A86A-1A44DAB896AD}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="4">
+      <c r="B1" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="2">
         <v>6</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <v>7</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="2">
         <v>8</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -572,7 +579,7 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -597,7 +604,7 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
@@ -612,7 +619,7 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
@@ -627,7 +634,7 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
@@ -642,7 +649,7 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
@@ -657,7 +664,7 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
@@ -672,7 +679,7 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
@@ -687,13 +694,13 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -712,7 +719,7 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -737,86 +744,92 @@
       <c r="K11" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
@@ -824,12 +837,6 @@
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>